<commit_message>
journal and draft model
</commit_message>
<xml_diff>
--- a/inputs/data/Conformed/SCAA_TastingNotes.xlsx
+++ b/inputs/data/Conformed/SCAA_TastingNotes.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Documents/GitHub/COFEE_COFFEE_COFFEE/inputs/data/Conformed/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Documents/GitHub/COFFEE_COFFEE_COFFEE/inputs/data/Conformed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD9239D-901D-8849-B5C6-10BBE3069A20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730DDF9B-A83A-9E4D-A6E3-5E36800099FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3800" yWindow="-18660" windowWidth="27880" windowHeight="16940" xr2:uid="{CC791C6D-82D9-2A4E-A8A1-BAA2B001B55E}"/>
+    <workbookView xWindow="3440" yWindow="-19320" windowWidth="27880" windowHeight="16940" xr2:uid="{CC791C6D-82D9-2A4E-A8A1-BAA2B001B55E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$268</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$321</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="334">
   <si>
     <t>Fruity</t>
   </si>
@@ -884,6 +884,162 @@
   <si>
     <t>Sugar Cane</t>
   </si>
+  <si>
+    <t>Chocolate Fudge</t>
+  </si>
+  <si>
+    <t>Fudge</t>
+  </si>
+  <si>
+    <t>Cherry Pie</t>
+  </si>
+  <si>
+    <t>Tart Cherry</t>
+  </si>
+  <si>
+    <t>Walnut</t>
+  </si>
+  <si>
+    <t>Key Lime</t>
+  </si>
+  <si>
+    <t>Roasty</t>
+  </si>
+  <si>
+    <t>Hot Cocoa</t>
+  </si>
+  <si>
+    <t>Hot Chocolate</t>
+  </si>
+  <si>
+    <t>Wild Berry</t>
+  </si>
+  <si>
+    <t>Meyer Lemon</t>
+  </si>
+  <si>
+    <t>Golden Raisin</t>
+  </si>
+  <si>
+    <t>Chocolate Éclair</t>
+  </si>
+  <si>
+    <t>Chocolate Eclair</t>
+  </si>
+  <si>
+    <t>White Peach</t>
+  </si>
+  <si>
+    <t>Toasted Nut</t>
+  </si>
+  <si>
+    <t>Ruby Red Grapefruit</t>
+  </si>
+  <si>
+    <t>White Grapefruit</t>
+  </si>
+  <si>
+    <t>Pink Grapefruit</t>
+  </si>
+  <si>
+    <t>Bartlett Pear</t>
+  </si>
+  <si>
+    <t>Grape Jam</t>
+  </si>
+  <si>
+    <t>Candied Orange</t>
+  </si>
+  <si>
+    <t>Raspberry Candy</t>
+  </si>
+  <si>
+    <t>Shortbread Cookie</t>
+  </si>
+  <si>
+    <t>Pine</t>
+  </si>
+  <si>
+    <t>Chardonnay</t>
+  </si>
+  <si>
+    <t>Pink Lady</t>
+  </si>
+  <si>
+    <t>Honeydew Melon</t>
+  </si>
+  <si>
+    <t>Black Grape</t>
+  </si>
+  <si>
+    <t>Honeycomb</t>
+  </si>
+  <si>
+    <t>Wild Cherry</t>
+  </si>
+  <si>
+    <t>Chocolate Mousse</t>
+  </si>
+  <si>
+    <t>Orange Zest</t>
+  </si>
+  <si>
+    <t>Lemon Zest</t>
+  </si>
+  <si>
+    <t>Lime Zest</t>
+  </si>
+  <si>
+    <t>Delicate</t>
+  </si>
+  <si>
+    <t>Dense</t>
+  </si>
+  <si>
+    <t>Redcurrant</t>
+  </si>
+  <si>
+    <t>Violet Candy</t>
+  </si>
+  <si>
+    <t>Guava</t>
+  </si>
+  <si>
+    <t>Mission Fig</t>
+  </si>
+  <si>
+    <t>Lemon Candy</t>
+  </si>
+  <si>
+    <t>Orange Candy</t>
+  </si>
+  <si>
+    <t>Lilac</t>
+  </si>
+  <si>
+    <t>Lavender Honey</t>
+  </si>
+  <si>
+    <t>Lavender</t>
+  </si>
+  <si>
+    <t>Rainier Cherry</t>
+  </si>
+  <si>
+    <t>Elegant</t>
+  </si>
+  <si>
+    <t>Clarity</t>
+  </si>
+  <si>
+    <t>Passionfruit</t>
+  </si>
+  <si>
+    <t>Passion Fruit</t>
+  </si>
+  <si>
+    <t>Forest Berry</t>
+  </si>
 </sst>
 </file>
 
@@ -1252,10 +1408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{022B90C7-7931-664C-97FF-ABC8E36BA1AA}">
-  <dimension ref="A1:XFD268"/>
+  <dimension ref="A1:XFD321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="H178" sqref="H178"/>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="G163" sqref="G163:G164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -66974,7 +67130,7 @@
         <v>195</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>269</v>
+        <v>317</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -66985,7 +67141,7 @@
         <v>195</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>270</v>
+        <v>329</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -66993,10 +67149,10 @@
         <v>3</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>192</v>
+        <v>330</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -67004,10 +67160,10 @@
         <v>3</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>193</v>
+        <v>318</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -67015,54 +67171,54 @@
         <v>3</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>9</v>
+        <v>195</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>9</v>
+        <v>201</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>255</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>9</v>
+        <v>201</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>271</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>9</v>
+        <v>201</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>254</v>
+        <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -67073,7 +67229,7 @@
         <v>9</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>9</v>
+        <v>278</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -67084,7 +67240,7 @@
         <v>9</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>10</v>
+        <v>255</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -67095,7 +67251,7 @@
         <v>9</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>11</v>
+        <v>271</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -67106,7 +67262,7 @@
         <v>9</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>12</v>
+        <v>254</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -67117,7 +67273,7 @@
         <v>9</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -67128,7 +67284,7 @@
         <v>9</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>272</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -67139,7 +67295,7 @@
         <v>9</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -67150,7 +67306,7 @@
         <v>9</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -67158,10 +67314,10 @@
         <v>7</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>279</v>
+        <v>9</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -67169,10 +67325,10 @@
         <v>7</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>279</v>
+        <v>9</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>20</v>
+        <v>272</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -67180,10 +67336,10 @@
         <v>7</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>279</v>
+        <v>9</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -67191,10 +67347,10 @@
         <v>7</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>279</v>
+        <v>9</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -67202,10 +67358,10 @@
         <v>7</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>16</v>
+        <v>279</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>16</v>
+        <v>307</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -67213,10 +67369,10 @@
         <v>7</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>16</v>
+        <v>279</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -67224,10 +67380,10 @@
         <v>7</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>16</v>
+        <v>279</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -67235,10 +67391,10 @@
         <v>7</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>16</v>
+        <v>279</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -67246,65 +67402,65 @@
         <v>7</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>16</v>
+        <v>279</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>164</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>27</v>
+        <v>164</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -67315,7 +67471,7 @@
         <v>24</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -67326,7 +67482,7 @@
         <v>24</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>29</v>
+        <v>292</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -67337,7 +67493,7 @@
         <v>24</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>147</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -67348,7 +67504,7 @@
         <v>24</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>148</v>
+        <v>323</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -67359,7 +67515,7 @@
         <v>24</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>151</v>
+        <v>324</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -67370,7 +67526,7 @@
         <v>24</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>152</v>
+        <v>303</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -67381,10 +67537,10 @@
         <v>24</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>246</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>0</v>
       </c>
@@ -67392,10 +67548,10 @@
         <v>24</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>247</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>0</v>
       </c>
@@ -67403,10 +67559,10 @@
         <v>24</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>215</v>
+        <v>287</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>0</v>
       </c>
@@ -67414,7 +67570,7 @@
         <v>24</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>216</v>
+        <v>27</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -67425,7 +67581,7 @@
         <v>24</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>165</v>
+        <v>314</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -67436,7 +67592,7 @@
         <v>24</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>197</v>
+        <v>315</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -67444,10 +67600,10 @@
         <v>0</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>280</v>
+        <v>316</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -67455,10 +67611,10 @@
         <v>0</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -67466,10 +67622,10 @@
         <v>0</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>273</v>
+        <v>29</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -67477,10 +67633,10 @@
         <v>0</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>231</v>
+        <v>298</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -67488,10 +67644,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>156</v>
+        <v>299</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -67499,10 +67655,10 @@
         <v>0</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>34</v>
+        <v>300</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -67510,10 +67666,10 @@
         <v>0</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>46</v>
+        <v>147</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -67521,10 +67677,10 @@
         <v>0</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>36</v>
+        <v>148</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -67532,10 +67688,10 @@
         <v>0</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>37</v>
+        <v>151</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -67543,43 +67699,43 @@
         <v>0</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>38</v>
+        <v>152</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>39</v>
+        <v>246</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>40</v>
+        <v>247</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>61</v>
+        <v>215</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -67587,10 +67743,10 @@
         <v>0</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>68</v>
+        <v>216</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -67598,10 +67754,10 @@
         <v>0</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>63</v>
+        <v>165</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -67609,10 +67765,10 @@
         <v>0</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>41</v>
+        <v>197</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -67623,7 +67779,7 @@
         <v>30</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>42</v>
+        <v>280</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -67634,7 +67790,7 @@
         <v>30</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -67645,7 +67801,7 @@
         <v>30</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>205</v>
+        <v>273</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -67656,7 +67812,7 @@
         <v>30</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>64</v>
+        <v>231</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -67667,10 +67823,10 @@
         <v>30</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>65</v>
+        <v>156</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>0</v>
       </c>
@@ -67678,10 +67834,10 @@
         <v>30</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>202</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>0</v>
       </c>
@@ -67689,10 +67845,10 @@
         <v>30</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>203</v>
+        <v>301</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>0</v>
       </c>
@@ -67700,10 +67856,10 @@
         <v>30</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>0</v>
       </c>
@@ -67711,10 +67867,10 @@
         <v>30</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>158</v>
+        <v>308</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>0</v>
       </c>
@@ -67722,10 +67878,10 @@
         <v>30</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>181</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>0</v>
       </c>
@@ -67733,10 +67889,10 @@
         <v>30</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>207</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>0</v>
       </c>
@@ -67744,10 +67900,10 @@
         <v>30</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>235</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>0</v>
       </c>
@@ -67755,10 +67911,10 @@
         <v>30</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>236</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>0</v>
       </c>
@@ -67766,10 +67922,10 @@
         <v>30</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>0</v>
       </c>
@@ -67777,10 +67933,10 @@
         <v>30</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>258</v>
+        <v>61</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>0</v>
       </c>
@@ -67788,10 +67944,10 @@
         <v>30</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>259</v>
+        <v>68</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>0</v>
       </c>
@@ -67799,10 +67955,10 @@
         <v>30</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>260</v>
+        <v>302</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>0</v>
       </c>
@@ -67810,10 +67966,10 @@
         <v>30</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>58</v>
+        <v>310</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>0</v>
       </c>
@@ -67821,393 +67977,407 @@
         <v>30</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H94" s="2"/>
-      <c r="I94" s="2"/>
+        <v>321</v>
+      </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="H95" s="2"/>
-      <c r="I95" s="2"/>
+        <v>63</v>
+      </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="H96" s="2"/>
-      <c r="I96" s="2"/>
+        <v>41</v>
+      </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="H97" s="2"/>
-      <c r="I97" s="2"/>
-      <c r="J97" s="2"/>
+        <v>309</v>
+      </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="H98" s="2"/>
-      <c r="I98" s="2"/>
-      <c r="J98" s="2"/>
+        <v>42</v>
+      </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>212</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>35</v>
+        <v>205</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>53</v>
+        <v>202</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>60</v>
+        <v>203</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>131</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>220</v>
+        <v>158</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>229</v>
+        <v>207</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>45</v>
+        <v>235</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>31</v>
+        <v>237</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>55</v>
+        <v>258</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>56</v>
+        <v>259</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>57</v>
+        <v>260</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>33</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="H115" s="2"/>
+      <c r="I115" s="2"/>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>217</v>
-      </c>
+        <v>322</v>
+      </c>
+      <c r="H116" s="2"/>
+      <c r="I116" s="2"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>331</v>
+      </c>
+      <c r="H117" s="2"/>
+      <c r="I117" s="2"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>218</v>
-      </c>
+        <v>332</v>
+      </c>
+      <c r="H118" s="2"/>
+      <c r="I118" s="2"/>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>219</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="H119" s="2"/>
+      <c r="I119" s="2"/>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>47</v>
-      </c>
+        <v>328</v>
+      </c>
+      <c r="H120" s="2"/>
+      <c r="I120" s="2"/>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>48</v>
-      </c>
+        <v>312</v>
+      </c>
+      <c r="H121" s="2"/>
+      <c r="I121" s="2"/>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>49</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="H122" s="2"/>
+      <c r="I122" s="2"/>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>50</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="H123" s="2"/>
+      <c r="I123" s="2"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>51</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="H124" s="2"/>
+      <c r="I124" s="2"/>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>62</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="H125" s="2"/>
+      <c r="I125" s="2"/>
+      <c r="J125" s="2"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>67</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="H126" s="2"/>
+      <c r="I126" s="2"/>
+      <c r="J126" s="2"/>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>136</v>
+        <v>211</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>245</v>
+        <v>212</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
@@ -68215,10 +68385,10 @@
         <v>0</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>137</v>
+        <v>296</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
@@ -68226,10 +68396,10 @@
         <v>0</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>138</v>
+        <v>35</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
@@ -68237,10 +68407,10 @@
         <v>0</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>139</v>
+        <v>44</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
@@ -68248,10 +68418,10 @@
         <v>0</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>140</v>
+        <v>52</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
@@ -68259,10 +68429,10 @@
         <v>0</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>153</v>
+        <v>53</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
@@ -68270,10 +68440,10 @@
         <v>0</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>154</v>
+        <v>60</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
@@ -68281,10 +68451,10 @@
         <v>0</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>240</v>
+        <v>131</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
@@ -68292,1466 +68462,2049 @@
         <v>0</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>257</v>
+        <v>220</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>208</v>
+        <v>157</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>249</v>
+        <v>45</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>163</v>
+        <v>232</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>155</v>
+        <v>293</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>141</v>
+        <v>57</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>135</v>
+        <v>291</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>134</v>
+        <v>33</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>129</v>
+        <v>218</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>69</v>
+        <v>219</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>222</v>
+        <v>304</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>223</v>
+        <v>47</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>204</v>
+        <v>49</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>130</v>
+        <v>50</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>162</v>
+        <v>51</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>214</v>
+        <v>62</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>250</v>
+        <v>67</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>251</v>
+        <v>136</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>149</v>
+        <v>245</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>2</v>
+        <v>137</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>187</v>
+        <v>138</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>177</v>
+        <v>319</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>241</v>
+        <v>139</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>242</v>
+        <v>140</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>244</v>
+        <v>153</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>73</v>
+        <v>154</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>75</v>
+        <v>33</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>168</v>
+        <v>240</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>75</v>
+        <v>33</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>74</v>
+        <v>333</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>75</v>
+        <v>33</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>75</v>
+        <v>257</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>76</v>
+        <v>208</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>77</v>
+        <v>326</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>78</v>
+        <v>327</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>79</v>
+        <v>248</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>80</v>
+        <v>249</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>133</v>
+        <v>163</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>142</v>
+        <v>70</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>143</v>
+        <v>249</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>144</v>
+        <v>71</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>76</v>
+        <v>1</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B182" s="1" t="s">
-        <v>76</v>
+        <v>1</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>281</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B183" s="1" t="s">
-        <v>76</v>
+        <v>1</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B184" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C184" s="1" t="s">
-        <v>185</v>
+        <v>1</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>325</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B185" s="1" t="s">
-        <v>76</v>
+        <v>1</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>179</v>
+        <v>141</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B186" s="1" t="s">
-        <v>76</v>
+        <v>1</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>180</v>
+        <v>135</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B187" s="1" t="s">
-        <v>76</v>
+        <v>1</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>182</v>
+        <v>134</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B188" s="1" t="s">
-        <v>76</v>
+        <v>1</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>261</v>
+        <v>221</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B189" s="1" t="s">
-        <v>76</v>
+        <v>1</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>262</v>
+        <v>70</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>81</v>
+        <v>1</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>243</v>
+        <v>129</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>81</v>
+        <v>1</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>230</v>
+        <v>69</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>183</v>
+        <v>222</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>184</v>
+        <v>223</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>145</v>
+        <v>204</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>82</v>
+        <v>130</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>83</v>
+        <v>162</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>5</v>
+        <v>72</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>84</v>
+        <v>214</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>5</v>
+        <v>72</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>85</v>
+        <v>250</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>5</v>
+        <v>72</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>86</v>
+        <v>251</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>146</v>
+        <v>2</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>5</v>
+        <v>187</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>186</v>
+        <v>305</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
     </row>
-    <row r="207" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C207" s="1" t="s">
-        <v>199</v>
+        <v>2</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>242</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C208" s="1" t="s">
-        <v>233</v>
+        <v>2</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>244</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C209" s="1" t="s">
-        <v>234</v>
+        <v>73</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="210" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C210" s="1" t="s">
-        <v>239</v>
+        <v>75</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>178</v>
+        <v>74</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>91</v>
+        <v>311</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>256</v>
+        <v>79</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>264</v>
+        <v>133</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A220" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>263</v>
+        <v>142</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>8</v>
+        <v>143</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A222" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A223" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B223" s="2" t="s">
-        <v>94</v>
+        <v>2</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>175</v>
+        <v>150</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A224" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B224" s="2" t="s">
-        <v>94</v>
+        <v>2</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>95</v>
+        <v>281</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B225" s="2" t="s">
-        <v>94</v>
+        <v>2</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>96</v>
+        <v>161</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B226" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C226" s="2" t="s">
-        <v>97</v>
+        <v>2</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B227" s="2" t="s">
-        <v>97</v>
+        <v>2</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B228" s="2" t="s">
-        <v>97</v>
+        <v>2</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>98</v>
+        <v>180</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B229" s="2" t="s">
-        <v>97</v>
+        <v>2</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>99</v>
+        <v>182</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B230" s="2" t="s">
-        <v>97</v>
+        <v>2</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>100</v>
+        <v>261</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B231" s="2" t="s">
-        <v>97</v>
+        <v>2</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>167</v>
+        <v>262</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>6</v>
+        <v>243</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A233" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="C233" s="2" t="s">
-        <v>101</v>
+        <v>230</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="C234" s="2" t="s">
-        <v>102</v>
+        <v>183</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A235" s="2" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>105</v>
+        <v>184</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236" s="2" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237" s="2" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>107</v>
+        <v>145</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A238" s="2" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239" s="2" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240" s="2" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>110</v>
+        <v>282</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241" s="2" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>112</v>
+        <v>283</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242" s="2" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>174</v>
+        <v>289</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243" s="2" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>173</v>
+        <v>294</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" s="2" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>113</v>
+        <v>295</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" s="2" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>169</v>
+        <v>290</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" s="2" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>170</v>
+        <v>313</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" s="2" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>111</v>
+        <v>5</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>171</v>
+        <v>286</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" s="2" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>111</v>
+        <v>5</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>172</v>
+        <v>84</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" s="2" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>111</v>
+        <v>5</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250" s="2" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>111</v>
+        <v>5</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251" s="2" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>111</v>
+        <v>5</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" s="2" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>111</v>
+        <v>5</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>117</v>
+        <v>146</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253" s="2" t="s">
-        <v>225</v>
+        <v>4</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>119</v>
+        <v>5</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>119</v>
+        <v>5</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254" s="2" t="s">
-        <v>225</v>
+        <v>4</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>118</v>
+        <v>5</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>224</v>
+        <v>297</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" s="2" t="s">
-        <v>225</v>
+        <v>4</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>118</v>
+        <v>5</v>
       </c>
       <c r="C255" s="2" t="s">
-        <v>226</v>
+        <v>159</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A256" s="2" t="s">
-        <v>225</v>
+        <v>4</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>118</v>
+        <v>5</v>
       </c>
       <c r="C256" s="2" t="s">
-        <v>227</v>
+        <v>186</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" s="2" t="s">
-        <v>225</v>
+        <v>4</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>118</v>
+        <v>5</v>
       </c>
       <c r="C257" s="2" t="s">
-        <v>228</v>
+        <v>252</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="2" t="s">
-        <v>225</v>
+        <v>4</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C258" s="2" t="s">
-        <v>160</v>
+        <v>5</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>199</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="2" t="s">
-        <v>225</v>
+        <v>4</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C259" s="2" t="s">
-        <v>120</v>
+        <v>5</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260" s="2" t="s">
-        <v>225</v>
+        <v>4</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C260" s="2" t="s">
-        <v>121</v>
+        <v>5</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261" s="2" t="s">
-        <v>225</v>
+        <v>4</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C261" s="2" t="s">
-        <v>122</v>
+        <v>5</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262" s="2" t="s">
-        <v>225</v>
+        <v>8</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>123</v>
+        <v>178</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263" s="2" t="s">
-        <v>225</v>
+        <v>8</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>124</v>
+        <v>88</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264" s="2" t="s">
-        <v>225</v>
+        <v>8</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>125</v>
+        <v>89</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A265" s="2" t="s">
-        <v>225</v>
+        <v>8</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="C265" s="2" t="s">
-        <v>126</v>
+        <v>90</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A266" s="2" t="s">
-        <v>225</v>
+        <v>8</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="C266" s="2" t="s">
-        <v>209</v>
+        <v>91</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267" s="2" t="s">
-        <v>225</v>
+        <v>8</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="C267" s="2" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B268" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C268" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A269" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B269" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C269" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A270" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B270" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C270" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A271" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B271" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A272" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B272" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A273" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B273" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A274" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B274" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A275" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B275" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A276" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B276" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C276" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A277" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B277" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A278" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B278" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A279" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B279" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A280" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B280" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A281" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B281" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A282" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B282" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C282" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A283" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B283" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C283" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A284" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B284" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C284" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A285" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B285" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C285" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A286" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B286" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C286" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A287" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B287" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C287" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A288" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B288" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C288" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A289" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B289" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C289" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A290" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B290" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C290" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A291" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B291" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C291" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A292" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B292" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C292" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A293" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B293" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C293" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A294" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B294" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C294" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A295" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B295" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C295" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A296" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B296" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C296" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A297" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B297" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C297" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A298" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B298" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C298" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A299" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B299" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C299" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A300" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B300" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C300" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A301" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B301" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C301" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A302" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B302" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C302" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A303" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B303" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C303" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A304" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B304" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C304" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A305" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B268" s="2" t="s">
+      <c r="B305" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C305" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A306" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B306" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C306" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A307" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B307" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C307" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A308" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B308" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C308" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A309" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B309" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C309" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A310" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B310" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C310" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A311" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B311" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C311" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A312" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B312" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C312" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A313" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B313" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C313" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A314" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B314" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C314" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A315" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B315" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C315" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A316" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B316" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C316" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A317" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B317" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C317" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A318" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B318" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C318" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A319" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B319" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C319" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A320" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B320" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C320" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A321" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B321" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C268" s="2" t="s">
+      <c r="C321" s="2" t="s">
         <v>128</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C268" xr:uid="{E1D67A3E-3F6F-7244-A79C-83B0D75C5BD3}"/>
+  <autoFilter ref="A1:C321" xr:uid="{E1D67A3E-3F6F-7244-A79C-83B0D75C5BD3}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>